<commit_message>
Update danh mục 3 thứ tiếng
</commit_message>
<xml_diff>
--- a/docs/Category/Danh muc update.xlsx
+++ b/docs/Category/Danh muc update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Topics</t>
   </si>
@@ -30,33 +30,9 @@
     <t>Level 3</t>
   </si>
   <si>
-    <t>Nước hoa quả - Juice</t>
-  </si>
-  <si>
-    <t>Bia rượu_x000D_ - Alcohol</t>
-  </si>
-  <si>
-    <t>Kẹo_x000D_ - Candy</t>
-  </si>
-  <si>
-    <t>Mứt_x000D_ - Jams</t>
-  </si>
-  <si>
-    <t>Bánh_x000D_ - Biscuits/Cakes</t>
-  </si>
-  <si>
-    <t>Dụng cụ vệ sinh_x000D_ - Hygiene</t>
-  </si>
-  <si>
-    <t>Đồ uống có ga_x000D_ - Carbonated</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
-    <t>Khăn / Đồ vải_x000D_ - Cloths/Towels - 패브릭 (Fabric)</t>
-  </si>
-  <si>
     <t>Thể thao_x000D_ - Sports - 스포츠</t>
   </si>
   <si>
@@ -69,9 +45,6 @@
     <t>Mẹ và bé - Mom &amp; Baby - 맘 &amp; 베이비</t>
   </si>
   <si>
-    <t>Tã &amp; dụng cụ vệ sinh_x000D_ - Diapering - 기저귀</t>
-  </si>
-  <si>
     <t>Đồ uống_x000D_ - Drinks - 음료</t>
   </si>
   <si>
@@ -135,9 +108,6 @@
     <t>Handmade_x000D_ - Handmade 수공예품</t>
   </si>
   <si>
-    <t>Thiệp cá nhân_x000D_ - Greeting Cards - 카드</t>
-  </si>
-  <si>
     <t>Made in Vietnam_x000D_ - Made in Vietnam - Made in Vietnam</t>
   </si>
   <si>
@@ -150,40 +120,67 @@
     <t>Phòng tắm/ngủ- Bath / Bed - 침구 / 욕실</t>
   </si>
   <si>
-    <t>Sản phẩm khác - Others</t>
-  </si>
-  <si>
     <t>Sản phẩm khác - Others - 기타</t>
   </si>
   <si>
-    <t>Phụ kiện / Ngủ - Accessories</t>
-  </si>
-  <si>
-    <t>Đồ ăn liền/hộp/khô_x000D_ - Instant/Cans/Dried</t>
-  </si>
-  <si>
-    <t>Bánh/kẹo/mứt_x000D_ - Sweetened</t>
-  </si>
-  <si>
-    <t>Đồ ăn khác_x000D_ - Other Foods</t>
-  </si>
-  <si>
     <t>Truyền thống_x000D_ - Cultural Clothes - 전통 의류</t>
   </si>
   <si>
-    <t>Đồ tặng khác - Other Gifts</t>
-  </si>
-  <si>
     <t>Trang trí - Décor - 데코</t>
   </si>
   <si>
-    <t>Đồ gia dụng - Home Living</t>
-  </si>
-  <si>
     <t>Bếp / Phòng ăn - Kitchen/Dinning - 주방</t>
   </si>
   <si>
     <t>Đồ chơi - Baby Toys - 아기 장난감</t>
+  </si>
+  <si>
+    <t>Đồ gia dụng - Home Living - 홈 리빙</t>
+  </si>
+  <si>
+    <t>Khăn / Đồ vải_x000D_ - Cloths/Towels - 패브릭 / 타월</t>
+  </si>
+  <si>
+    <t>Dụng cụ vệ sinh_x000D_ - Hygiene - 위생</t>
+  </si>
+  <si>
+    <t>Phụ kiện / Ngủ - Accessories - 액세서리</t>
+  </si>
+  <si>
+    <t>Đồ ăn liền/hộp/khô_x000D_ - Instant/Cans/Dried - 인스턴트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước hoa quả - Juice - 주스 </t>
+  </si>
+  <si>
+    <t>Bia rượu_x000D_ - Alcohol - 술</t>
+  </si>
+  <si>
+    <t>Đồ uống có ga_x000D_ - Carbonated - 탄산음료</t>
+  </si>
+  <si>
+    <t>Bánh/kẹo/mứt_x000D_ - Sweetened - 과자</t>
+  </si>
+  <si>
+    <t>Bánh_x000D_ - Biscuits/Cakes - 과자</t>
+  </si>
+  <si>
+    <t>Kẹo_x000D_ - Candy- 사탕</t>
+  </si>
+  <si>
+    <t>Mứt_x000D_ - Jams - 잼</t>
+  </si>
+  <si>
+    <t>Đồ ăn khác_x000D_ - Other Foods - 기타</t>
+  </si>
+  <si>
+    <t>Thiệp cá nhân_x000D_ - Greeting Cards - 인사 카드</t>
+  </si>
+  <si>
+    <t>Đồ tặng khác - Other Gifts - 기타</t>
+  </si>
+  <si>
+    <t>Tã/ Vệ sinh_x000D_ - Diapering - 기저귀</t>
   </si>
 </sst>
 </file>
@@ -224,8 +221,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -270,8 +266,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -283,6 +279,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -577,9 +576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,13 +600,13 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="C2" s="6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -629,7 +628,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -640,7 +639,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -651,7 +650,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -661,7 +660,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="5" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -671,7 +670,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -681,7 +680,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -691,7 +690,7 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -701,7 +700,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -711,7 +710,7 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -720,7 +719,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -730,8 +729,8 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>17</v>
+      <c r="C15" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -742,7 +741,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -752,7 +751,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -761,7 +760,7 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -771,7 +770,7 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -782,7 +781,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -792,7 +791,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -802,7 +801,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -812,7 +811,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -822,7 +821,7 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -831,7 +830,7 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -841,7 +840,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -851,7 +850,7 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -861,7 +860,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -870,7 +869,7 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -881,7 +880,7 @@
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -892,7 +891,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -902,7 +901,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -912,7 +911,7 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -921,7 +920,7 @@
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -932,7 +931,7 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -942,7 +941,7 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -952,7 +951,7 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -962,7 +961,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -972,7 +971,7 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -981,7 +980,7 @@
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -992,7 +991,7 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1002,7 +1001,7 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1012,7 +1011,7 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -1022,7 +1021,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -1031,7 +1030,7 @@
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1041,7 +1040,7 @@
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1051,7 +1050,7 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1060,7 +1059,7 @@
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1071,7 +1070,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="5" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1081,7 +1080,7 @@
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1091,7 +1090,7 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1101,7 +1100,7 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1110,7 +1109,7 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1120,7 +1119,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>

</xml_diff>